<commit_message>
[UPDATE][FEATURE] REGRE ENQ Y  NUEVOS CASOS DE DEPOSITOS EN EFEC
[UPDATE] Regresion ENQ TEST-9522

[FEATURE] Se crearon nuevos casos de Depositos en efectivo por caja,
DEC11-17
</commit_message>
<xml_diff>
--- a/Test Data/User.xlsx
+++ b/Test Data/User.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017287A0-A309-44B1-922F-C47F05A46356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19998F5-7034-4960-B866-DC7980CB9CEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>User</t>
   </si>
@@ -457,9 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -645,6 +647,14 @@
         <v>38</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>